<commit_message>
RVC and MVS initial cleaning
Finished script for creating MVS_Start.csv and RVC_Start.csv.
</commit_message>
<xml_diff>
--- a/Data_SmallFiles/Fish/MVS-RVC_SpeciesCodes_Dictionary.xlsx
+++ b/Data_SmallFiles/Fish/MVS-RVC_SpeciesCodes_Dictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
   <si>
     <t>OLD_MVS_CODE</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>URO_JAMA</t>
+  </si>
+  <si>
+    <t>SPH_BORE</t>
+  </si>
+  <si>
+    <t>SYN_FLOR</t>
+  </si>
+  <si>
+    <t>SYN_LOUI</t>
+  </si>
+  <si>
+    <t>TRI_INSC</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,6 +1891,9 @@
       <c r="A54" t="s">
         <v>105</v>
       </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -2180,6 +2195,9 @@
       <c r="A92" t="s">
         <v>177</v>
       </c>
+      <c r="B92" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
@@ -2273,11 +2291,17 @@
       <c r="A104" t="s">
         <v>199</v>
       </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>200</v>
       </c>
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -2290,6 +2314,9 @@
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>203</v>
+      </c>
+      <c r="B107" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed scripts regarding biomass and density.
MaxEnt modelling will not include density occurrence records, niche density, or predator biomass so those scripts were removed (archived in GoogleDrive).
</commit_message>
<xml_diff>
--- a/Data_SmallFiles/Fish/MVS-RVC_SpeciesCodes_Dictionary.xlsx
+++ b/Data_SmallFiles/Fish/MVS-RVC_SpeciesCodes_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="MVS_Code_Dictionary" sheetId="1" r:id="rId1"/>
@@ -1457,11 +1457,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>